<commit_message>
Added logic to map revenue codes in IBMs
</commit_message>
<xml_diff>
--- a/docs/IBM_CCAE_MDCR/images/Defining_VISIT_DETAIL_Examples.xlsx
+++ b/docs/IBM_CCAE_MDCR/images/Defining_VISIT_DETAIL_Examples.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1E27172-5346-4BED-9216-AD704A658F51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairblacketer/Documents/GitHub/ETL-LambdaBuilder/docs/IBM_CCAE_MDCR/images/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D1A7D0-F215-944E-811E-3D390D4419BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29180" yWindow="1480" windowWidth="29060" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exampl1" sheetId="1" r:id="rId1"/>
@@ -99,9 +104,6 @@
     <t>ER</t>
   </si>
   <si>
-    <t xml:space="preserve">(1) Those lines of claims above are from one inpatient admission in inpatient_services table (enrolid = 10422705, caseid = 19971). The first 2 lines are ER claims (identified by PROC1 = 99285, STDPLAC =23, REVCODE = '0450')with SVCDATE one day before the ADMATE of this inpatient visit.  Thus this inpatient admission defined by Truven can be divided into one ER visit and one IP visit. </t>
-  </si>
-  <si>
     <t xml:space="preserve">(1)Those lines of claim above are from outpatient_services table
 (2) Lines 6 and 7 are inpatient claims (REVCODE ='0120' and '0121'),  and they can be consolidated as one inpatient visit.  Line 2 is an ER claim (PROC1 ='99284'), thus it is defined an ER visit since it falls on the Visit_Start_Date of the inpatient visit.  Other line of claims fall between the start and end dates of the inpatient visit, thus are considered as part of it.
 </t>
@@ -141,6 +143,9 @@
   </si>
   <si>
     <t>OP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) Those lines of claims above are from one inpatient admission in inpatient_services table (enrolid = 10422705, caseid = 19971). The first 2 lines are ER claims (identified by STDPLAC =23) with SVCDATE one day before the ADMATE of this inpatient visit.  Thus this inpatient admission defined by Truven can be divided into one ER visit and one IP visit. </t>
   </si>
 </sst>
 </file>
@@ -832,7 +837,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -848,10 +853,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1311,48 +1312,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="2"/>
+    <col min="12" max="12" width="9.1640625" style="2"/>
     <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" customWidth="1"/>
+    <col min="17" max="17" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.33203125" customWidth="1"/>
     <col min="19" max="19" width="11.6640625" customWidth="1"/>
-    <col min="20" max="20" width="12.88671875" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" customWidth="1"/>
     <col min="21" max="21" width="10.6640625" customWidth="1"/>
-    <col min="22" max="22" width="14.44140625" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" customWidth="1"/>
+    <col min="23" max="23" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11.33203125" customWidth="1"/>
-    <col min="27" max="27" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="S2" s="59" t="s">
+    <row r="2" spans="2:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="57"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
+      <c r="W2" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="60"/>
-    </row>
-    <row r="3" spans="2:27" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+    </row>
+    <row r="3" spans="2:27" ht="48" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1401,38 +1402,38 @@
       <c r="Q3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="S3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="18" t="s">
+      <c r="T3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="U3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="27" t="s">
+      <c r="V3" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="X3" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y3" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z3" s="34" t="s">
+      <c r="AA3" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B4" s="7">
         <v>40178</v>
       </c>
@@ -1457,7 +1458,7 @@
       <c r="I4" s="8">
         <v>29650</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="47">
         <v>99285</v>
       </c>
       <c r="K4" s="8">
@@ -1469,7 +1470,7 @@
       <c r="M4" s="8">
         <v>477727</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="11">
         <v>23</v>
       </c>
       <c r="O4" s="8" t="s">
@@ -1481,10 +1482,10 @@
       <c r="Q4" s="8">
         <v>30220</v>
       </c>
-      <c r="R4" s="15">
+      <c r="R4" s="13">
         <v>40177</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="17">
         <v>1</v>
       </c>
       <c r="T4" s="7">
@@ -1493,10 +1494,10 @@
       <c r="U4" s="7">
         <v>40177</v>
       </c>
-      <c r="V4" s="28" t="s">
+      <c r="V4" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="36">
+      <c r="W4" s="34">
         <v>1</v>
       </c>
       <c r="X4" s="10">
@@ -1508,11 +1509,11 @@
       <c r="Z4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="37">
+      <c r="AA4" s="35">
         <v>1234</v>
       </c>
     </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B5" s="7">
         <v>40178</v>
       </c>
@@ -1537,19 +1538,19 @@
       <c r="I5" s="8">
         <v>29650</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="47">
         <v>99285</v>
       </c>
       <c r="K5" s="8">
         <v>364008243</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="9">
         <v>450</v>
       </c>
       <c r="M5" s="8">
         <v>477728</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="11">
         <v>23</v>
       </c>
       <c r="O5" s="8">
@@ -1561,10 +1562,10 @@
       <c r="Q5" s="8">
         <v>30120</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R5" s="13">
         <v>40177</v>
       </c>
-      <c r="S5" s="19">
+      <c r="S5" s="17">
         <v>1</v>
       </c>
       <c r="T5" s="7">
@@ -1573,10 +1574,10 @@
       <c r="U5" s="7">
         <v>40177</v>
       </c>
-      <c r="V5" s="28" t="s">
+      <c r="V5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="W5" s="36">
+      <c r="W5" s="34">
         <v>2</v>
       </c>
       <c r="X5" s="10">
@@ -1588,11 +1589,11 @@
       <c r="Z5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="37">
+      <c r="AA5" s="35">
         <v>5678</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B6" s="10">
         <v>40178</v>
       </c>
@@ -1641,10 +1642,10 @@
       <c r="Q6" s="4">
         <v>30330</v>
       </c>
-      <c r="R6" s="16">
-        <v>40178</v>
-      </c>
-      <c r="S6" s="20">
+      <c r="R6" s="14">
+        <v>40178</v>
+      </c>
+      <c r="S6" s="18">
         <v>2</v>
       </c>
       <c r="T6" s="10">
@@ -1653,10 +1654,10 @@
       <c r="U6" s="10">
         <v>40181</v>
       </c>
-      <c r="V6" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="38">
+      <c r="V6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W6" s="36">
         <v>3</v>
       </c>
       <c r="X6" s="10">
@@ -1668,11 +1669,11 @@
       <c r="Z6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA6" s="37">
+      <c r="AA6" s="35">
         <v>3456</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B7" s="10">
         <v>40178</v>
       </c>
@@ -1721,10 +1722,10 @@
       <c r="Q7" s="4">
         <v>30399</v>
       </c>
-      <c r="R7" s="16">
-        <v>40178</v>
-      </c>
-      <c r="S7" s="20">
+      <c r="R7" s="14">
+        <v>40178</v>
+      </c>
+      <c r="S7" s="18">
         <v>2</v>
       </c>
       <c r="T7" s="10">
@@ -1733,10 +1734,10 @@
       <c r="U7" s="10">
         <v>40181</v>
       </c>
-      <c r="V7" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W7" s="38">
+      <c r="V7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W7" s="36">
         <v>4</v>
       </c>
       <c r="X7" s="10">
@@ -1748,11 +1749,11 @@
       <c r="Z7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA7" s="39">
+      <c r="AA7" s="37">
         <v>7890</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B8" s="10">
         <v>40178</v>
       </c>
@@ -1801,10 +1802,10 @@
       <c r="Q8" s="4">
         <v>30399</v>
       </c>
-      <c r="R8" s="16">
-        <v>40178</v>
-      </c>
-      <c r="S8" s="20">
+      <c r="R8" s="14">
+        <v>40178</v>
+      </c>
+      <c r="S8" s="18">
         <v>2</v>
       </c>
       <c r="T8" s="10">
@@ -1813,11 +1814,11 @@
       <c r="U8" s="10">
         <v>40181</v>
       </c>
-      <c r="V8" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W8" s="38">
-        <v>4</v>
+      <c r="V8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W8" s="36">
+        <v>5</v>
       </c>
       <c r="X8" s="10">
         <v>40177</v>
@@ -1828,11 +1829,11 @@
       <c r="Z8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA8" s="39">
+      <c r="AA8" s="37">
         <v>7890</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B9" s="10">
         <v>40178</v>
       </c>
@@ -1881,10 +1882,10 @@
       <c r="Q9" s="4">
         <v>30110</v>
       </c>
-      <c r="R9" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S9" s="20">
+      <c r="R9" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S9" s="18">
         <v>2</v>
       </c>
       <c r="T9" s="10">
@@ -1893,11 +1894,11 @@
       <c r="U9" s="10">
         <v>40181</v>
       </c>
-      <c r="V9" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W9" s="38">
-        <v>5</v>
+      <c r="V9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W9" s="36">
+        <v>6</v>
       </c>
       <c r="X9" s="10">
         <v>40177</v>
@@ -1908,11 +1909,11 @@
       <c r="Z9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA9" s="39">
+      <c r="AA9" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B10" s="10">
         <v>40178</v>
       </c>
@@ -1961,10 +1962,10 @@
       <c r="Q10" s="4">
         <v>30110</v>
       </c>
-      <c r="R10" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S10" s="20">
+      <c r="R10" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S10" s="18">
         <v>2</v>
       </c>
       <c r="T10" s="10">
@@ -1973,11 +1974,11 @@
       <c r="U10" s="10">
         <v>40181</v>
       </c>
-      <c r="V10" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W10" s="38">
-        <v>5</v>
+      <c r="V10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W10" s="36">
+        <v>7</v>
       </c>
       <c r="X10" s="10">
         <v>40177</v>
@@ -1988,11 +1989,11 @@
       <c r="Z10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA10" s="39">
+      <c r="AA10" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B11" s="10">
         <v>40178</v>
       </c>
@@ -2041,10 +2042,10 @@
       <c r="Q11" s="4">
         <v>30134</v>
       </c>
-      <c r="R11" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S11" s="20">
+      <c r="R11" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S11" s="18">
         <v>2</v>
       </c>
       <c r="T11" s="10">
@@ -2053,11 +2054,11 @@
       <c r="U11" s="10">
         <v>40181</v>
       </c>
-      <c r="V11" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W11" s="38">
-        <v>5</v>
+      <c r="V11" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W11" s="36">
+        <v>8</v>
       </c>
       <c r="X11" s="10">
         <v>40177</v>
@@ -2068,11 +2069,11 @@
       <c r="Z11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA11" s="39">
+      <c r="AA11" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B12" s="10">
         <v>40178</v>
       </c>
@@ -2121,10 +2122,10 @@
       <c r="Q12" s="4">
         <v>30159</v>
       </c>
-      <c r="R12" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S12" s="20">
+      <c r="R12" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S12" s="18">
         <v>2</v>
       </c>
       <c r="T12" s="10">
@@ -2133,11 +2134,11 @@
       <c r="U12" s="10">
         <v>40181</v>
       </c>
-      <c r="V12" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W12" s="38">
-        <v>5</v>
+      <c r="V12" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W12" s="36">
+        <v>9</v>
       </c>
       <c r="X12" s="10">
         <v>40177</v>
@@ -2148,11 +2149,11 @@
       <c r="Z12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA12" s="39">
+      <c r="AA12" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B13" s="10">
         <v>40178</v>
       </c>
@@ -2201,10 +2202,10 @@
       <c r="Q13" s="4">
         <v>30152</v>
       </c>
-      <c r="R13" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S13" s="20">
+      <c r="R13" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S13" s="18">
         <v>2</v>
       </c>
       <c r="T13" s="10">
@@ -2213,11 +2214,11 @@
       <c r="U13" s="10">
         <v>40181</v>
       </c>
-      <c r="V13" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W13" s="38">
-        <v>5</v>
+      <c r="V13" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W13" s="36">
+        <v>10</v>
       </c>
       <c r="X13" s="10">
         <v>40177</v>
@@ -2228,11 +2229,11 @@
       <c r="Z13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA13" s="39">
+      <c r="AA13" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B14" s="10">
         <v>40178</v>
       </c>
@@ -2281,10 +2282,10 @@
       <c r="Q14" s="4">
         <v>30134</v>
       </c>
-      <c r="R14" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S14" s="20">
+      <c r="R14" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S14" s="18">
         <v>2</v>
       </c>
       <c r="T14" s="10">
@@ -2293,11 +2294,11 @@
       <c r="U14" s="10">
         <v>40181</v>
       </c>
-      <c r="V14" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W14" s="38">
-        <v>5</v>
+      <c r="V14" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W14" s="36">
+        <v>11</v>
       </c>
       <c r="X14" s="10">
         <v>40177</v>
@@ -2308,11 +2309,11 @@
       <c r="Z14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA14" s="39">
+      <c r="AA14" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B15" s="10">
         <v>40178</v>
       </c>
@@ -2361,10 +2362,10 @@
       <c r="Q15" s="4">
         <v>30134</v>
       </c>
-      <c r="R15" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S15" s="20">
+      <c r="R15" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S15" s="18">
         <v>2</v>
       </c>
       <c r="T15" s="10">
@@ -2373,11 +2374,11 @@
       <c r="U15" s="10">
         <v>40181</v>
       </c>
-      <c r="V15" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W15" s="38">
-        <v>5</v>
+      <c r="V15" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W15" s="36">
+        <v>12</v>
       </c>
       <c r="X15" s="10">
         <v>40177</v>
@@ -2388,11 +2389,11 @@
       <c r="Z15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA15" s="39">
+      <c r="AA15" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B16" s="10">
         <v>40178</v>
       </c>
@@ -2441,10 +2442,10 @@
       <c r="Q16" s="4">
         <v>30151</v>
       </c>
-      <c r="R16" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S16" s="20">
+      <c r="R16" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S16" s="18">
         <v>2</v>
       </c>
       <c r="T16" s="10">
@@ -2453,11 +2454,11 @@
       <c r="U16" s="10">
         <v>40181</v>
       </c>
-      <c r="V16" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W16" s="38">
-        <v>5</v>
+      <c r="V16" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W16" s="36">
+        <v>13</v>
       </c>
       <c r="X16" s="10">
         <v>40177</v>
@@ -2468,11 +2469,11 @@
       <c r="Z16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA16" s="39">
+      <c r="AA16" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B17" s="10">
         <v>40178</v>
       </c>
@@ -2521,10 +2522,10 @@
       <c r="Q17" s="4">
         <v>30134</v>
       </c>
-      <c r="R17" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S17" s="20">
+      <c r="R17" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S17" s="18">
         <v>2</v>
       </c>
       <c r="T17" s="10">
@@ -2533,11 +2534,11 @@
       <c r="U17" s="10">
         <v>40181</v>
       </c>
-      <c r="V17" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W17" s="38">
-        <v>5</v>
+      <c r="V17" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W17" s="36">
+        <v>14</v>
       </c>
       <c r="X17" s="10">
         <v>40177</v>
@@ -2548,11 +2549,11 @@
       <c r="Z17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA17" s="39">
+      <c r="AA17" s="37">
         <v>2233</v>
       </c>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B18" s="10">
         <v>40178</v>
       </c>
@@ -2601,10 +2602,10 @@
       <c r="Q18" s="4">
         <v>30226</v>
       </c>
-      <c r="R18" s="16">
+      <c r="R18" s="14">
         <v>40179</v>
       </c>
-      <c r="S18" s="20">
+      <c r="S18" s="18">
         <v>2</v>
       </c>
       <c r="T18" s="10">
@@ -2613,11 +2614,11 @@
       <c r="U18" s="10">
         <v>40181</v>
       </c>
-      <c r="V18" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W18" s="38">
-        <v>6</v>
+      <c r="V18" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W18" s="36">
+        <v>15</v>
       </c>
       <c r="X18" s="10">
         <v>40179</v>
@@ -2628,11 +2629,11 @@
       <c r="Z18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA18" s="39">
+      <c r="AA18" s="37">
         <v>4747</v>
       </c>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B19" s="10">
         <v>40178</v>
       </c>
@@ -2681,10 +2682,10 @@
       <c r="Q19" s="4">
         <v>30226</v>
       </c>
-      <c r="R19" s="16">
+      <c r="R19" s="14">
         <v>40179</v>
       </c>
-      <c r="S19" s="20">
+      <c r="S19" s="18">
         <v>2</v>
       </c>
       <c r="T19" s="10">
@@ -2693,11 +2694,11 @@
       <c r="U19" s="10">
         <v>40181</v>
       </c>
-      <c r="V19" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W19" s="38">
-        <v>7</v>
+      <c r="V19" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W19" s="36">
+        <v>16</v>
       </c>
       <c r="X19" s="10">
         <v>40179</v>
@@ -2708,11 +2709,11 @@
       <c r="Z19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA19" s="37">
+      <c r="AA19" s="35">
         <v>3456</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B20" s="10">
         <v>40178</v>
       </c>
@@ -2761,10 +2762,10 @@
       <c r="Q20" s="4">
         <v>30226</v>
       </c>
-      <c r="R20" s="16">
+      <c r="R20" s="14">
         <v>40180</v>
       </c>
-      <c r="S20" s="20">
+      <c r="S20" s="18">
         <v>2</v>
       </c>
       <c r="T20" s="10">
@@ -2773,11 +2774,11 @@
       <c r="U20" s="10">
         <v>40181</v>
       </c>
-      <c r="V20" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W20" s="38">
-        <v>8</v>
+      <c r="V20" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W20" s="36">
+        <v>17</v>
       </c>
       <c r="X20" s="10">
         <v>40180</v>
@@ -2788,11 +2789,11 @@
       <c r="Z20" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA20" s="39">
+      <c r="AA20" s="37">
         <v>4747</v>
       </c>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B21" s="10">
         <v>40178</v>
       </c>
@@ -2841,10 +2842,10 @@
       <c r="Q21" s="4">
         <v>30226</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R21" s="14">
         <v>40180</v>
       </c>
-      <c r="S21" s="20">
+      <c r="S21" s="18">
         <v>2</v>
       </c>
       <c r="T21" s="10">
@@ -2853,11 +2854,11 @@
       <c r="U21" s="10">
         <v>40181</v>
       </c>
-      <c r="V21" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W21" s="38">
-        <v>9</v>
+      <c r="V21" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W21" s="36">
+        <v>18</v>
       </c>
       <c r="X21" s="10">
         <v>40180</v>
@@ -2868,11 +2869,11 @@
       <c r="Z21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA21" s="37">
+      <c r="AA21" s="35">
         <v>3456</v>
       </c>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B22" s="10">
         <v>40178</v>
       </c>
@@ -2921,10 +2922,10 @@
       <c r="Q22" s="4">
         <v>30226</v>
       </c>
-      <c r="R22" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S22" s="20">
+      <c r="R22" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S22" s="18">
         <v>2</v>
       </c>
       <c r="T22" s="10">
@@ -2933,11 +2934,11 @@
       <c r="U22" s="10">
         <v>40181</v>
       </c>
-      <c r="V22" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="W22" s="38">
-        <v>10</v>
+      <c r="V22" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="W22" s="36">
+        <v>19</v>
       </c>
       <c r="X22" s="10">
         <v>40181</v>
@@ -2948,11 +2949,11 @@
       <c r="Z22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA22" s="39">
+      <c r="AA22" s="37">
         <v>4747</v>
       </c>
     </row>
-    <row r="23" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10">
         <v>40178</v>
       </c>
@@ -3001,118 +3002,118 @@
       <c r="Q23" s="4">
         <v>30226</v>
       </c>
-      <c r="R23" s="16">
-        <v>40181</v>
-      </c>
-      <c r="S23" s="21">
+      <c r="R23" s="14">
+        <v>40181</v>
+      </c>
+      <c r="S23" s="19">
         <v>2</v>
       </c>
-      <c r="T23" s="22">
-        <v>40178</v>
-      </c>
-      <c r="U23" s="22">
-        <v>40181</v>
-      </c>
-      <c r="V23" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="W23" s="40">
-        <v>11</v>
-      </c>
-      <c r="X23" s="22">
-        <v>40181</v>
-      </c>
-      <c r="Y23" s="22">
-        <v>40181</v>
-      </c>
-      <c r="Z23" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA23" s="46">
+      <c r="T23" s="20">
+        <v>40178</v>
+      </c>
+      <c r="U23" s="20">
+        <v>40181</v>
+      </c>
+      <c r="V23" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="W23" s="38">
+        <v>20</v>
+      </c>
+      <c r="X23" s="20">
+        <v>40181</v>
+      </c>
+      <c r="Y23" s="20">
+        <v>40181</v>
+      </c>
+      <c r="Z23" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA23" s="44">
         <v>3456</v>
       </c>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B25" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="58"/>
-      <c r="S26" s="58"/>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B25" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="56"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="56"/>
+      <c r="S25" s="56"/>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="56"/>
+      <c r="R26" s="56"/>
+      <c r="S26" s="56"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="56"/>
+      <c r="S27" s="56"/>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3133,117 +3134,117 @@
       <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="1"/>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" customWidth="1"/>
+    <col min="16" max="16" width="11.1640625" customWidth="1"/>
     <col min="17" max="17" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.33203125" customWidth="1"/>
-    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-    </row>
-    <row r="3" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="23" t="s">
+    <row r="2" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+    </row>
+    <row r="3" spans="1:24" ht="48" x14ac:dyDescent="0.2">
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="N3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="18" t="s">
+      <c r="P3" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="27" t="s">
+      <c r="R3" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="U3" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="S3" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="V3" s="34" t="s">
+      <c r="W3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="W3" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="35" t="s">
+      <c r="X3" s="33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B4" s="7">
         <v>4660</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="29">
         <v>30516604</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <v>99284</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -3255,7 +3256,7 @@
       <c r="I4" s="8">
         <v>53374966</v>
       </c>
-      <c r="J4" s="49">
+      <c r="J4" s="47">
         <v>22</v>
       </c>
       <c r="K4" s="8">
@@ -3267,10 +3268,10 @@
       <c r="M4" s="8">
         <v>21120</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="13">
         <v>38409</v>
       </c>
-      <c r="O4" s="19">
+      <c r="O4" s="17">
         <v>1</v>
       </c>
       <c r="P4" s="7">
@@ -3279,10 +3280,10 @@
       <c r="Q4" s="7">
         <v>38409</v>
       </c>
-      <c r="R4" s="15" t="s">
+      <c r="R4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="S4" s="36">
+      <c r="S4" s="34">
         <v>1</v>
       </c>
       <c r="T4" s="10">
@@ -3297,19 +3298,19 @@
       <c r="W4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="37">
+      <c r="X4" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
-      <c r="B5" s="51">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49">
         <v>4660</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="30">
         <v>30516604</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -3327,34 +3328,34 @@
       <c r="I5" s="3">
         <v>53374965</v>
       </c>
-      <c r="J5" s="52">
+      <c r="J5" s="50">
         <v>21</v>
       </c>
       <c r="K5" s="3">
         <v>240</v>
       </c>
-      <c r="L5" s="51">
+      <c r="L5" s="49">
         <v>38409</v>
       </c>
       <c r="M5" s="3">
         <v>22130</v>
       </c>
-      <c r="N5" s="54">
+      <c r="N5" s="52">
         <v>38409</v>
       </c>
-      <c r="O5" s="53">
+      <c r="O5" s="51">
         <v>2</v>
       </c>
-      <c r="P5" s="51">
+      <c r="P5" s="49">
         <v>38409</v>
       </c>
-      <c r="Q5" s="51">
+      <c r="Q5" s="49">
         <v>38413</v>
       </c>
-      <c r="R5" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="S5" s="38">
+      <c r="R5" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" s="36">
         <v>2</v>
       </c>
       <c r="T5" s="10">
@@ -3364,23 +3365,23 @@
         <v>38409</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X5" s="56">
+      <c r="X5" s="54">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B6" s="10">
         <v>4660</v>
       </c>
       <c r="C6" s="4">
         <v>7580</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="41">
         <v>30516604</v>
       </c>
       <c r="E6" s="4">
@@ -3392,8 +3393,8 @@
       <c r="G6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="47" t="s">
-        <v>39</v>
+      <c r="H6" s="45" t="s">
+        <v>38</v>
       </c>
       <c r="I6" s="4">
         <v>53374967</v>
@@ -3410,10 +3411,10 @@
       <c r="M6" s="4">
         <v>10510</v>
       </c>
-      <c r="N6" s="16">
+      <c r="N6" s="14">
         <v>38413</v>
       </c>
-      <c r="O6" s="44">
+      <c r="O6" s="42">
         <v>2</v>
       </c>
       <c r="P6" s="10">
@@ -3422,10 +3423,10 @@
       <c r="Q6" s="10">
         <v>38413</v>
       </c>
-      <c r="R6" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="S6" s="38">
+      <c r="R6" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" s="36">
         <v>3</v>
       </c>
       <c r="T6" s="10">
@@ -3435,23 +3436,23 @@
         <v>38413</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X6" s="56">
+      <c r="X6" s="54">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B7" s="10">
         <v>4660</v>
       </c>
       <c r="C7" s="4">
         <v>7580</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="41">
         <v>30516604</v>
       </c>
       <c r="E7" s="4">
@@ -3481,10 +3482,10 @@
       <c r="M7" s="4">
         <v>10599</v>
       </c>
-      <c r="N7" s="16">
+      <c r="N7" s="14">
         <v>38413</v>
       </c>
-      <c r="O7" s="44">
+      <c r="O7" s="42">
         <v>2</v>
       </c>
       <c r="P7" s="10">
@@ -3493,10 +3494,10 @@
       <c r="Q7" s="10">
         <v>38413</v>
       </c>
-      <c r="R7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="S7" s="38">
+      <c r="R7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S7" s="36">
         <v>3</v>
       </c>
       <c r="T7" s="10">
@@ -3506,23 +3507,23 @@
         <v>38413</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X7" s="56">
+      <c r="X7" s="54">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B8" s="7">
         <v>4660</v>
       </c>
       <c r="C8" s="8">
         <v>7580</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="29">
         <v>30516604</v>
       </c>
       <c r="E8" s="8">
@@ -3534,13 +3535,13 @@
       <c r="G8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="48" t="s">
-        <v>37</v>
+      <c r="H8" s="46" t="s">
+        <v>36</v>
       </c>
       <c r="I8" s="8">
         <v>53374963</v>
       </c>
-      <c r="J8" s="49">
+      <c r="J8" s="47">
         <v>21</v>
       </c>
       <c r="K8" s="8">
@@ -3552,10 +3553,10 @@
       <c r="M8" s="8">
         <v>10510</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="13">
         <v>38413</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="17">
         <v>2</v>
       </c>
       <c r="P8" s="7">
@@ -3564,10 +3565,10 @@
       <c r="Q8" s="7">
         <v>38413</v>
       </c>
-      <c r="R8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="S8" s="38">
+      <c r="R8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="S8" s="36">
         <v>4</v>
       </c>
       <c r="T8" s="10">
@@ -3582,18 +3583,18 @@
       <c r="W8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X8" s="56">
+      <c r="X8" s="54">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B9" s="7">
         <v>4660</v>
       </c>
       <c r="C9" s="8">
         <v>7580</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="29">
         <v>30516604</v>
       </c>
       <c r="E9" s="8">
@@ -3605,13 +3606,13 @@
       <c r="G9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="48" t="s">
-        <v>38</v>
+      <c r="H9" s="46" t="s">
+        <v>37</v>
       </c>
       <c r="I9" s="8">
         <v>53374964</v>
       </c>
-      <c r="J9" s="49">
+      <c r="J9" s="47">
         <v>21</v>
       </c>
       <c r="K9" s="8">
@@ -3623,10 +3624,10 @@
       <c r="M9" s="8">
         <v>10510</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="13">
         <v>38413</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="17">
         <v>2</v>
       </c>
       <c r="P9" s="7">
@@ -3635,10 +3636,10 @@
       <c r="Q9" s="7">
         <v>38413</v>
       </c>
-      <c r="R9" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="S9" s="38">
+      <c r="R9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="S9" s="36">
         <v>4</v>
       </c>
       <c r="T9" s="10">
@@ -3653,18 +3654,18 @@
       <c r="W9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X9" s="56">
+      <c r="X9" s="54">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B10" s="10">
         <v>4660</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="43">
+      <c r="D10" s="41">
         <v>30516604</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -3694,10 +3695,10 @@
       <c r="M10" s="4">
         <v>20161</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="14">
         <v>38411</v>
       </c>
-      <c r="O10" s="44">
+      <c r="O10" s="42">
         <v>2</v>
       </c>
       <c r="P10" s="10">
@@ -3706,10 +3707,10 @@
       <c r="Q10" s="10">
         <v>38413</v>
       </c>
-      <c r="R10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="S10" s="38">
+      <c r="R10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S10" s="36">
         <v>5</v>
       </c>
       <c r="T10" s="10">
@@ -3719,23 +3720,23 @@
         <v>38411</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X10" s="56">
+      <c r="X10" s="54">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B11" s="10">
         <v>486</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="41">
         <v>30516604</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -3765,10 +3766,10 @@
       <c r="M11" s="4">
         <v>20226</v>
       </c>
-      <c r="N11" s="16">
+      <c r="N11" s="14">
         <v>38411</v>
       </c>
-      <c r="O11" s="44">
+      <c r="O11" s="42">
         <v>2</v>
       </c>
       <c r="P11" s="10">
@@ -3777,10 +3778,10 @@
       <c r="Q11" s="10">
         <v>38413</v>
       </c>
-      <c r="R11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="S11" s="38">
+      <c r="R11" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="S11" s="36">
         <v>5</v>
       </c>
       <c r="T11" s="10">
@@ -3790,23 +3791,23 @@
         <v>38411</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="X11" s="56">
+      <c r="X11" s="54">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>486</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="41">
         <v>30516604</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -3836,117 +3837,117 @@
       <c r="M12" s="4">
         <v>20226</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="14">
         <v>38413</v>
       </c>
-      <c r="O12" s="45">
+      <c r="O12" s="43">
         <v>2</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="20">
         <v>38409</v>
       </c>
-      <c r="Q12" s="22">
+      <c r="Q12" s="20">
         <v>38413</v>
       </c>
-      <c r="R12" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="S12" s="40">
+      <c r="R12" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="S12" s="38">
         <v>6</v>
       </c>
-      <c r="T12" s="22">
+      <c r="T12" s="20">
         <v>38413</v>
       </c>
-      <c r="U12" s="22">
+      <c r="U12" s="20">
         <v>38413</v>
       </c>
-      <c r="V12" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="W12" s="57" t="s">
+      <c r="V12" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="W12" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="X12" s="42">
+      <c r="X12" s="40">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B14" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="58"/>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="58"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="58"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="58"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
-      <c r="L16" s="58"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="58"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="58"/>
-      <c r="Q16" s="58"/>
-      <c r="R16" s="58"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="58"/>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B14" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B16" s="56"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>